<commit_message>
updated week 9 and 10 status tracker
</commit_message>
<xml_diff>
--- a/docs/StatusTracker_week8.xlsx
+++ b/docs/StatusTracker_week8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinitmehta/Desktop/IIITH/Sem4/DASS/Project/dass-project-spring-2024-team-41/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA51DCE4-974C-7940-90D1-5FC5E53AEF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772CB8D3-E619-734B-A040-ED025DC794F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="149">
   <si>
     <t>Using the Status tracker</t>
   </si>
@@ -484,9 +484,6 @@
     <t>Display other drone status info</t>
   </si>
   <si>
-    <t>Week 9 (March 18 - March 25)</t>
-  </si>
-  <si>
     <t>Manasa</t>
   </si>
   <si>
@@ -527,6 +524,48 @@
   </si>
   <si>
     <t>GPS reading of user</t>
+  </si>
+  <si>
+    <t>Week 9 (March 18 - March 24)</t>
+  </si>
+  <si>
+    <t>Week 10 (March 25 - March 31)</t>
+  </si>
+  <si>
+    <t>Set on hold for now because client has to communicate some config info</t>
+  </si>
+  <si>
+    <t>Telemetry to be displayed in header</t>
+  </si>
+  <si>
+    <t>Change in Action Menu</t>
+  </si>
+  <si>
+    <t>Map Full screen mode in settings</t>
+  </si>
+  <si>
+    <t>Video Feed Button</t>
+  </si>
+  <si>
+    <t>Meeting with client</t>
+  </si>
+  <si>
+    <t>Vinit, Medha</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Week 11 (April 1 - April 7)</t>
+  </si>
+  <si>
+    <t>Quiz 2</t>
+  </si>
+  <si>
+    <t>Ready Button Back End</t>
+  </si>
+  <si>
+    <t>Ready Button Front End</t>
   </si>
 </sst>
 </file>
@@ -1251,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I232"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
@@ -1606,7 +1645,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="H16" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2167,7 +2206,7 @@
         <v>2</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="H36" s="20">
         <f t="shared" si="0"/>
@@ -2542,7 +2581,7 @@
         <v>84</v>
       </c>
       <c r="C51" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D51" s="1">
         <v>2</v>
@@ -2579,7 +2618,7 @@
         <v>15</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="H52" s="20">
         <f t="shared" si="2"/>
@@ -2638,7 +2677,7 @@
         <v>37</v>
       </c>
       <c r="H54" s="20">
-        <f>IF(OR(D54="", E54=""), "", D54-E54)</f>
+        <f t="shared" ref="H54:H69" si="4">IF(OR(D54="", E54=""), "", D54-E54)</f>
         <v>-7</v>
       </c>
       <c r="I54" s="20">
@@ -2666,11 +2705,11 @@
         <v>37</v>
       </c>
       <c r="H55" s="20">
-        <f>IF(OR(D55="", E55=""), "", D55-E55)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I55" s="20">
-        <f>IF(OR(H55="",E55=0),"",ABS(H55)/E55*100)</f>
+        <f t="shared" ref="I55:I64" si="5">IF(OR(H55="",E55=0),"",ABS(H55)/E55*100)</f>
         <v>0</v>
       </c>
     </row>
@@ -2694,11 +2733,11 @@
         <v>37</v>
       </c>
       <c r="H56" s="20">
-        <f>IF(OR(D56="", E56=""), "", D56-E56)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I56" s="20">
-        <f>IF(OR(H56="",E56=0),"",ABS(H56)/E56*100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2722,11 +2761,11 @@
         <v>37</v>
       </c>
       <c r="H57" s="20">
-        <f>IF(OR(D57="", E57=""), "", D57-E57)</f>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="I57" s="20">
-        <f>IF(OR(H57="",E57=0),"",ABS(H57)/E57*100)</f>
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
     </row>
@@ -2750,11 +2789,11 @@
         <v>37</v>
       </c>
       <c r="H58" s="20">
-        <f>IF(OR(D58="", E58=""), "", D58-E58)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I58" s="20">
-        <f>IF(OR(H58="",E58=0),"",ABS(H58)/E58*100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2778,11 +2817,11 @@
         <v>37</v>
       </c>
       <c r="H59" s="20">
-        <f>IF(OR(D59="", E59=""), "", D59-E59)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I59" s="20">
-        <f>IF(OR(H59="",E59=0),"",ABS(H59)/E59*100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2797,11 +2836,11 @@
       <c r="F60" s="19"/>
       <c r="G60" s="16"/>
       <c r="H60" s="20" t="str">
-        <f>IF(OR(D60="", E60=""), "", D60-E60)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I60" s="20" t="str">
-        <f>IF(OR(H60="",E60=0),"",ABS(H60)/E60*100)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -2813,7 +2852,7 @@
         <v>84</v>
       </c>
       <c r="C61" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D61" s="1">
         <v>2</v>
@@ -2825,11 +2864,11 @@
         <v>55</v>
       </c>
       <c r="H61" s="20">
-        <f>IF(OR(D61="", E61=""), "", D61-E61)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I61" s="20">
-        <f>IF(OR(H61="",E61=0),"",ABS(H61)/E61*100)</f>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
     </row>
@@ -2838,7 +2877,7 @@
         <v>117</v>
       </c>
       <c r="B62" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C62" s="29" t="s">
         <v>42</v>
@@ -2853,11 +2892,11 @@
         <v>37</v>
       </c>
       <c r="H62" s="20">
-        <f>IF(OR(D62="", E62=""), "", D62-E62)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I62" s="20">
-        <f>IF(OR(H62="",E62=0),"",ABS(H62)/E62*100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2881,11 +2920,11 @@
         <v>37</v>
       </c>
       <c r="H63" s="20">
-        <f>IF(OR(D63="", E63=""), "", D63-E63)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I63" s="20">
-        <f>IF(OR(H63="",E63=0),"",ABS(H63)/E63*100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2906,14 +2945,14 @@
         <v>2</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="H64" s="20">
-        <f>IF(OR(D64="", E64=""), "", D64-E64)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I64" s="20">
-        <f>IF(OR(H64="",E64=0),"",ABS(H64)/E64*100)</f>
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
     </row>
@@ -2937,17 +2976,17 @@
         <v>37</v>
       </c>
       <c r="H65" s="20">
-        <f>IF(OR(D65="", E65=""), "", D65-E65)</f>
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
       <c r="I65" s="20">
-        <f t="shared" ref="I65:I99" si="4">IF(OR(H65="",E65=0),"",ABS(H65)/E65*100)</f>
+        <f t="shared" ref="I65:I99" si="6">IF(OR(H65="",E65=0),"",ABS(H65)/E65*100)</f>
         <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A66" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B66" t="s">
         <v>84</v>
@@ -2965,7 +3004,7 @@
         <v>37</v>
       </c>
       <c r="H66" s="20">
-        <f>IF(OR(D66="", E66=""), "", D66-E66)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I66" s="20">
@@ -2975,7 +3014,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A67" s="30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B67" t="s">
         <v>49</v>
@@ -2990,10 +3029,10 @@
         <v>3</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="H67" s="20">
-        <f>IF(OR(D67="", E67=""), "", D67-E67)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I67" s="20">
@@ -3003,7 +3042,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A68" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B68" t="s">
         <v>84</v>
@@ -3018,13 +3057,13 @@
         <v>6</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="G68" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H68" s="20">
-        <f>IF(OR(D68="", E68=""), "", D68-E68)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I68" s="20">
@@ -3034,31 +3073,31 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A69" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B69" t="s">
         <v>84</v>
       </c>
       <c r="C69" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D69" s="1">
         <v>2</v>
       </c>
       <c r="E69" s="29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>55</v>
       </c>
       <c r="G69" s="30"/>
       <c r="H69" s="20">
-        <f>IF(OR(D69="", E69=""), "", D69-E69)</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>-2</v>
       </c>
       <c r="I69" s="20">
         <f>IF(OR(H69="",E69=0),"",ABS(H69)/E69*100)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.15">
@@ -3081,20 +3120,20 @@
         <v>37</v>
       </c>
       <c r="G70" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H70" s="20">
-        <f t="shared" ref="H70:H99" si="5">IF(OR(D70="", E70=""), "", D70-E70)</f>
+        <f t="shared" ref="H70:H99" si="7">IF(OR(D70="", E70=""), "", D70-E70)</f>
         <v>-2</v>
       </c>
       <c r="I70" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>66.666666666666657</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A71" s="28" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="B71" s="16"/>
       <c r="C71" s="17"/>
@@ -3113,10 +3152,10 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A72" s="30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B72" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C72" s="29" t="s">
         <v>42</v>
@@ -3124,24 +3163,24 @@
       <c r="D72" s="1">
         <v>1</v>
       </c>
-      <c r="E72" s="1" t="s">
-        <v>116</v>
+      <c r="E72" s="1">
+        <v>15</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H72" s="20" t="e">
+        <v>37</v>
+      </c>
+      <c r="H72" s="20">
         <f>IF(OR(D72="", E72=""), "", D72-E72)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I72" s="20" t="e">
+        <v>-14</v>
+      </c>
+      <c r="I72" s="20">
         <f>IF(OR(H72="",E72=0),"",ABS(H72)/E72*100)</f>
-        <v>#VALUE!</v>
+        <v>93.333333333333329</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A73" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B73" t="s">
         <v>101</v>
@@ -3152,19 +3191,19 @@
       <c r="D73" s="1">
         <v>5</v>
       </c>
-      <c r="E73" s="1" t="s">
-        <v>116</v>
+      <c r="E73" s="1">
+        <v>5</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H73" s="20" t="e">
+        <v>37</v>
+      </c>
+      <c r="H73" s="20">
         <f>IF(OR(D73="", E73=""), "", D73-E73)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I73" s="20" t="e">
+        <v>0</v>
+      </c>
+      <c r="I73" s="20">
         <f>IF(OR(H73="",E73=0),"",ABS(H73)/E73*100)</f>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.15">
@@ -3180,24 +3219,24 @@
       <c r="D74" s="1">
         <v>1</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>116</v>
+      <c r="E74" s="1">
+        <v>1</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H74" s="20" t="e">
+        <v>37</v>
+      </c>
+      <c r="H74" s="20">
         <f>IF(OR(D74="", E74=""), "", D74-E74)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I74" s="20" t="e">
+        <v>0</v>
+      </c>
+      <c r="I74" s="20">
         <f>IF(OR(H74="",E74=0),"",ABS(H74)/E74*100)</f>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A75" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B75" t="s">
         <v>84</v>
@@ -3208,1578 +3247,1758 @@
       <c r="D75" s="1">
         <v>10</v>
       </c>
-      <c r="E75" s="1" t="s">
-        <v>116</v>
+      <c r="E75" s="1">
+        <v>4</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H75" s="20" t="e">
+        <v>55</v>
+      </c>
+      <c r="G75" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="H75" s="20">
         <f>IF(OR(D75="", E75=""), "", D75-E75)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I75" s="20" t="e">
+        <v>6</v>
+      </c>
+      <c r="I75" s="20">
         <f>IF(OR(H75="",E75=0),"",ABS(H75)/E75*100)</f>
-        <v>#VALUE!</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A76" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B76" t="s">
         <v>84</v>
       </c>
       <c r="C76" s="29" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="D76" s="1">
         <v>4</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="E76" s="1">
+        <v>2</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H76" s="20">
+        <f t="shared" ref="H76" si="8">IF(OR(D76="", E76=""), "", D76-E76)</f>
+        <v>2</v>
+      </c>
+      <c r="I76" s="20">
+        <f t="shared" ref="I76" si="9">IF(OR(H76="",E76=0),"",ABS(H76)/E76*100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A77" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B77" s="16"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="20" t="str">
+        <f t="shared" ref="H77:H86" si="10">IF(OR(D77="", E77=""), "", D77-E77)</f>
+        <v/>
+      </c>
+      <c r="I77" s="20" t="str">
+        <f t="shared" ref="I77:I86" si="11">IF(OR(H77="",E77=0),"",ABS(H77)/E77*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A78" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" t="s">
+        <v>84</v>
+      </c>
+      <c r="C78" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
+      <c r="E78" s="1">
+        <v>1</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H78" s="20">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I78" s="20">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A79" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="B79" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C79" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D79" s="1">
+        <v>2</v>
+      </c>
+      <c r="E79" s="1">
+        <v>1</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H79" s="20">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="I79" s="20">
+        <f t="shared" si="11"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A80" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="B80" t="s">
+        <v>84</v>
+      </c>
+      <c r="C80" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D80" s="1">
+        <v>2</v>
+      </c>
+      <c r="E80" s="1">
+        <v>5</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H80" s="20">
+        <f t="shared" si="10"/>
+        <v>-3</v>
+      </c>
+      <c r="I80" s="20">
+        <f t="shared" si="11"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A81" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="B81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="D81" s="1">
+        <v>4</v>
+      </c>
+      <c r="E81" s="1">
+        <v>4</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H81" s="20">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I81" s="20">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A82" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="B82" t="s">
+        <v>84</v>
+      </c>
+      <c r="C82" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D82" s="1">
+        <v>2</v>
+      </c>
+      <c r="E82" s="1">
+        <v>4</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H82" s="20">
+        <f t="shared" si="10"/>
+        <v>-2</v>
+      </c>
+      <c r="I82" s="20">
+        <f t="shared" si="11"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A83" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="B83" t="s">
+        <v>35</v>
+      </c>
+      <c r="C83" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D83" s="1">
+        <v>5</v>
+      </c>
+      <c r="E83" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F76" s="4" t="s">
+      <c r="F83" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H76" s="20" t="e">
-        <f t="shared" ref="H76" si="6">IF(OR(D76="", E76=""), "", D76-E76)</f>
+      <c r="G83" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="H83" s="20" t="e">
+        <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I76" s="20" t="e">
-        <f t="shared" ref="I76" si="7">IF(OR(H76="",E76=0),"",ABS(H76)/E76*100)</f>
+      <c r="I83" s="20" t="e">
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H77" s="20" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I77" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H78" s="20" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I78" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H79" s="20" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I79" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H80" s="20" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I80" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.15">
-      <c r="H81" s="20" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I81" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.15">
-      <c r="H82" s="20" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I82" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.15">
-      <c r="H83" s="20" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I83" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.15">
-      <c r="H84" s="20" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I84" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A84" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B84" t="s">
+        <v>49</v>
+      </c>
+      <c r="C84" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D84" s="1">
+        <v>1</v>
+      </c>
+      <c r="E84" s="1">
+        <v>1</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H84" s="20">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I84" s="20">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A85" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="B85" s="16"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="17"/>
+      <c r="F85" s="19"/>
+      <c r="G85" s="16"/>
       <c r="H85" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="H85" si="12">IF(OR(D85="", E85=""), "", D85-E85)</f>
         <v/>
       </c>
       <c r="I85" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.15">
-      <c r="H86" s="20" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I86" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.15">
-      <c r="H87" s="20" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I87" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" ref="I85" si="13">IF(OR(H85="",E85=0),"",ABS(H85)/E85*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A86" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C86" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D86" s="1">
+        <v>20</v>
+      </c>
+      <c r="E86" s="1">
+        <v>20</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H86" s="20">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I86" s="20">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A87" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="C87" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D87" s="1">
+        <v>2</v>
+      </c>
+      <c r="E87" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H87" s="20" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I87" s="20" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H88" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I88" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H89" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I89" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H90" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I90" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H91" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I91" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H92" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I92" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H93" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I93" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H94" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I94" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H95" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I95" s="20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H96" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I96" s="20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H97" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I97" s="20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="98" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H98" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I98" s="20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="99" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H99" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I99" s="20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="100" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H100" s="20" t="str">
-        <f t="shared" ref="H100:H131" si="8">IF(OR(D100="", E100=""), "", D100-E100)</f>
+        <f t="shared" ref="H100:H131" si="14">IF(OR(D100="", E100=""), "", D100-E100)</f>
         <v/>
       </c>
       <c r="I100" s="20" t="str">
-        <f t="shared" ref="I100:I131" si="9">IF(OR(H100="",E100=0),"",ABS(H100)/E100*100)</f>
+        <f t="shared" ref="I100:I131" si="15">IF(OR(H100="",E100=0),"",ABS(H100)/E100*100)</f>
         <v/>
       </c>
     </row>
     <row r="101" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H101" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I101" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="102" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H102" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I102" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="103" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H103" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I103" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="104" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H104" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I104" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="105" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H105" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I105" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="106" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H106" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I106" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H107" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I107" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H108" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I108" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="109" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H109" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I109" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="110" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H110" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I110" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="111" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H111" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I111" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="112" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H112" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I112" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="113" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H113" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I113" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="114" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H114" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I114" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="115" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H115" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I115" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="116" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H116" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I116" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="117" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H117" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I117" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="118" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H118" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I118" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="119" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H119" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I119" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="120" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H120" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I120" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="121" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H121" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I121" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="122" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H122" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I122" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="123" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H123" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I123" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="124" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H124" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I124" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="125" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H125" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I125" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="126" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H126" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I126" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="127" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H127" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I127" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="128" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H128" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I128" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="129" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H129" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I129" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="130" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H130" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I130" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="131" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H131" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I131" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="132" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H132" s="20" t="str">
-        <f t="shared" ref="H132:H163" si="10">IF(OR(D132="", E132=""), "", D132-E132)</f>
+        <f t="shared" ref="H132:H163" si="16">IF(OR(D132="", E132=""), "", D132-E132)</f>
         <v/>
       </c>
       <c r="I132" s="20" t="str">
-        <f t="shared" ref="I132:I163" si="11">IF(OR(H132="",E132=0),"",ABS(H132)/E132*100)</f>
+        <f t="shared" ref="I132:I163" si="17">IF(OR(H132="",E132=0),"",ABS(H132)/E132*100)</f>
         <v/>
       </c>
     </row>
     <row r="133" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H133" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I133" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="134" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H134" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I134" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="135" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H135" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I135" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="136" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H136" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I136" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="137" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H137" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I137" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="138" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H138" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I138" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="139" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H139" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I139" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="140" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H140" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I140" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="141" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H141" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I141" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="142" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H142" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I142" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="143" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H143" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I143" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="144" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H144" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I144" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="145" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H145" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I145" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="146" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H146" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I146" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="147" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H147" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I147" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="148" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H148" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I148" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="149" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H149" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I149" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="150" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H150" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I150" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="151" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H151" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I151" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="152" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H152" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I152" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="153" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H153" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I153" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="154" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H154" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I154" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="155" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H155" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I155" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="156" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H156" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I156" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="157" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H157" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I157" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="158" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H158" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I158" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="159" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H159" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I159" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="160" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H160" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I160" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="161" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H161" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I161" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="162" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H162" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I162" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="163" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H163" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I163" s="20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="164" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H164" s="20" t="str">
-        <f t="shared" ref="H164:H195" si="12">IF(OR(D164="", E164=""), "", D164-E164)</f>
+        <f t="shared" ref="H164:H195" si="18">IF(OR(D164="", E164=""), "", D164-E164)</f>
         <v/>
       </c>
       <c r="I164" s="20" t="str">
-        <f t="shared" ref="I164:I195" si="13">IF(OR(H164="",E164=0),"",ABS(H164)/E164*100)</f>
+        <f t="shared" ref="I164:I195" si="19">IF(OR(H164="",E164=0),"",ABS(H164)/E164*100)</f>
         <v/>
       </c>
     </row>
     <row r="165" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H165" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I165" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="166" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H166" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I166" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="167" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H167" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I167" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="168" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H168" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I168" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="169" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H169" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I169" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="170" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H170" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I170" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="171" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H171" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I171" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="172" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H172" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I172" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="173" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H173" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I173" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="174" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H174" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I174" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="175" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H175" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I175" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="176" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H176" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I176" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="177" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H177" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I177" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="178" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H178" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I178" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="179" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H179" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I179" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="180" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H180" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I180" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="181" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H181" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I181" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="182" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H182" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I182" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="183" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H183" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I183" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="184" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H184" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I184" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="185" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H185" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I185" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="186" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H186" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I186" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="187" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H187" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I187" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="188" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H188" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I188" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="189" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H189" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I189" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="190" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H190" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I190" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="191" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H191" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I191" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="192" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H192" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I192" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="193" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H193" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I193" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="194" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H194" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I194" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="195" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H195" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I195" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="196" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H196" s="20" t="str">
-        <f t="shared" ref="H196:H225" si="14">IF(OR(D196="", E196=""), "", D196-E196)</f>
+        <f t="shared" ref="H196:H225" si="20">IF(OR(D196="", E196=""), "", D196-E196)</f>
         <v/>
       </c>
       <c r="I196" s="20" t="str">
-        <f t="shared" ref="I196:I227" si="15">IF(OR(H196="",E196=0),"",ABS(H196)/E196*100)</f>
+        <f t="shared" ref="I196:I227" si="21">IF(OR(H196="",E196=0),"",ABS(H196)/E196*100)</f>
         <v/>
       </c>
     </row>
     <row r="197" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H197" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I197" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="198" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H198" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I198" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="199" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H199" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I199" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="200" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H200" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I200" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="201" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H201" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I201" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="202" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H202" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I202" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="203" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H203" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I203" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="204" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H204" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I204" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="205" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H205" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I205" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="206" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H206" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I206" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="207" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H207" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I207" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="208" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H208" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I208" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="209" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H209" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I209" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="210" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H210" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I210" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="211" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H211" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I211" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="212" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H212" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I212" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="213" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H213" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I213" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="214" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H214" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I214" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="215" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H215" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I215" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="216" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H216" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I216" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="217" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H217" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I217" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="218" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H218" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I218" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="219" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H219" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I219" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="220" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H220" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I220" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="221" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H221" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I221" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="222" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H222" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I222" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="223" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H223" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I223" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="224" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H224" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I224" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="225" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H225" s="20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I225" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="226" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I226" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="227" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I227" s="20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="228" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I228" s="20" t="str">
-        <f t="shared" ref="I228:I259" si="16">IF(OR(H228="",E228=0),"",ABS(H228)/E228*100)</f>
+        <f t="shared" ref="I228:I232" si="22">IF(OR(H228="",E228=0),"",ABS(H228)/E228*100)</f>
         <v/>
       </c>
     </row>
     <row r="229" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I229" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
     <row r="230" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I230" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
     <row r="231" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I231" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
     <row r="232" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I232" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
@@ -4800,7 +5019,7 @@
       <formula1>"Planned,Ongoing,Delayed,Done"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B1232" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B78 B80:B1232" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Requirements,Design,Development,Testing,Preparation,Coordination,Documentation,Interfaces,Delivery"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>